<commit_message>
Update news and publication
</commit_message>
<xml_diff>
--- a/script/faculty_info.xlsx
+++ b/script/faculty_info.xlsx
@@ -56,83 +56,83 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>郑岩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yan Zheng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Siqi Chen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>职位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>研究方向</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>个人主页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>照片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Associate Professor, College of Intelligence and Computing, Tianjin University</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiagent Systems; Deep Reinforcement Learning; Evolutionary Algorithm; </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Artificial Intelligence, Multiagent systems, Game theory, Human-agent Interaction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.icdai.org/jianye.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://yanzzzzz.github.io/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈锶奇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://cic.tju.edu.cn/info/1072/1170.htm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deep Reinforcement Learning; Representation Learning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Artificial intelligence; Multi-agent systems; Machine Learning; Game Theroy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Postdoc at University of Alberta</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Postdoctoral Fellow of UdeM/MILA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>郑岩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yan Zheng</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Siqi Chen</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>姓名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>英文名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>职位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>研究方向</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>个人主页</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>照片</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Associate Professor, College of Intelligence and Computing, Tianjin University</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiagent Systems; Deep Reinforcement Learning; Evolutionary Algorithm; </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Artificial Intelligence, Multiagent systems, Game theory, Human-agent Interaction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://www.icdai.org/jianye.html</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://yanzzzzz.github.io/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>陈锶奇</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>http://cic.tju.edu.cn/info/1072/1170.htm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deep Reinforcement Learning; Representation Learning</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Artificial intelligence; Multi-agent systems; Machine Learning; Game Theroy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -480,7 +480,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -496,22 +496,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -522,47 +522,47 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -573,7 +573,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>6</v>
@@ -593,10 +593,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>2</v>

</xml_diff>